<commit_message>
Add implementation of OCA Validator
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -800,46 +800,43 @@
     <t xml:space="preserve">OL: Entry Code Mapping</t>
   </si>
   <si>
-    <t xml:space="preserve">first_name</t>
+    <t xml:space="preserve">email*</t>
   </si>
   <si>
     <t xml:space="preserve">utf-8</t>
   </si>
   <si>
-    <t xml:space="preserve">[a-zA-Z]+</t>
+    <t xml:space="preserve">[^@ \t\r\n]+@[^@ \t\r\n]+\.[^@ \t\r\n]+</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">last_name</t>
+    <t xml:space="preserve">licenses*</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t xml:space="preserve">A|B|C|D|E</t>
   </si>
   <si>
-    <t xml:space="preserve">age</t>
+    <t xml:space="preserve">number</t>
   </si>
   <si>
-    <t xml:space="preserve">sex</t>
+    <t xml:space="preserve">numbers</t>
   </si>
   <si>
-    <t xml:space="preserve">M|F|X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth_date</t>
+    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">DD.MM.YYYY</t>
   </si>
   <si>
-    <t xml:space="preserve">cities</t>
+    <t xml:space="preserve">dates</t>
   </si>
   <si>
-    <t xml:space="preserve">licenses</t>
+    <t xml:space="preserve">bool</t>
   </si>
   <si>
-    <t xml:space="preserve">A|B|C|D|E|F</t>
+    <t xml:space="preserve">bools</t>
   </si>
   <si>
     <t xml:space="preserve">Issuer</t>
@@ -2425,9 +2422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>117000</xdr:colOff>
+      <xdr:colOff>115560</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2441,7 +2438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4061520" y="282960"/>
-          <a:ext cx="2896920" cy="817200"/>
+          <a:ext cx="2895480" cy="815760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4177,7 +4174,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4266,7 +4263,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" s="72" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="72" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="61"/>
       <c r="B4" s="62" t="s">
         <v>91</v>
@@ -4313,18 +4310,16 @@
         <v>95</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>96</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D5" s="64"/>
       <c r="E5" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66" t="s">
+        <v>96</v>
+      </c>
       <c r="H5" s="67"/>
       <c r="I5" s="66"/>
       <c r="J5" s="68"/>
@@ -4393,16 +4388,14 @@
         <v>98</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D7" s="64"/>
       <c r="E7" s="65" t="s">
         <v>92</v>
       </c>
       <c r="F7" s="66"/>
-      <c r="G7" s="66" t="s">
-        <v>99</v>
-      </c>
+      <c r="G7" s="66"/>
       <c r="H7" s="67"/>
       <c r="I7" s="66"/>
       <c r="J7" s="68"/>
@@ -4429,7 +4422,7 @@
         <v/>
       </c>
       <c r="B8" s="67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="74" t="s">
         <v>60</v>
@@ -4439,7 +4432,7 @@
         <v>92</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" s="66"/>
       <c r="H8" s="67"/>
@@ -4468,25 +4461,23 @@
         <v/>
       </c>
       <c r="B9" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D9" s="64"/>
       <c r="E9" s="65" t="s">
         <v>92</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="67"/>
       <c r="I9" s="66"/>
       <c r="J9" s="68"/>
-      <c r="K9" s="70" t="s">
-        <v>94</v>
-      </c>
+      <c r="K9" s="70"/>
       <c r="L9" s="75"/>
       <c r="M9" s="75"/>
       <c r="N9" s="75"/>
@@ -4509,19 +4500,17 @@
         <v/>
       </c>
       <c r="B10" s="67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" s="64"/>
       <c r="E10" s="65" t="s">
         <v>92</v>
       </c>
       <c r="F10" s="66"/>
-      <c r="G10" s="66" t="s">
-        <v>104</v>
-      </c>
+      <c r="G10" s="0"/>
       <c r="H10" s="67"/>
       <c r="I10" s="66"/>
       <c r="J10" s="68"/>
@@ -4547,10 +4536,16 @@
         <f aca="false">IF(AND(NOT(ISBLANK(A$4)),NOT($B11="")),A$4,"")</f>
         <v/>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="78"/>
+      <c r="B11" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>55</v>
+      </c>
       <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
+      <c r="E11" s="65" t="s">
+        <v>92</v>
+      </c>
       <c r="F11" s="66"/>
       <c r="G11" s="66"/>
       <c r="H11" s="67"/>
@@ -35326,6 +35321,7 @@
       <c r="Z1003" s="76"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <conditionalFormatting sqref="C4:C1003">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(ISBLANK(C4),NOT(ISBLANK(B4)))</formula>
@@ -35414,10 +35410,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F1" s="86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -35446,10 +35442,10 @@
       <c r="C2" s="88"/>
       <c r="D2" s="55"/>
       <c r="E2" s="89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -35474,10 +35470,10 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="91" t="s">
         <v>107</v>
-      </c>
-      <c r="B3" s="91" t="s">
-        <v>108</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>22</v>
@@ -35517,7 +35513,7 @@
       <c r="B4" s="93"/>
       <c r="C4" s="94" t="str">
         <f aca="false">IF(ISBLANK(Main!$B4),"",Main!$B4)</f>
-        <v>first_name</v>
+        <v>email*</v>
       </c>
       <c r="D4" s="95"/>
       <c r="E4" s="96"/>
@@ -35534,7 +35530,7 @@
       </c>
       <c r="C5" s="73" t="str">
         <f aca="false">IF(ISBLANK(Main!$B5),"",Main!$B5)</f>
-        <v>last_name</v>
+        <v>licenses*</v>
       </c>
       <c r="D5" s="99"/>
       <c r="E5" s="100"/>
@@ -35551,7 +35547,7 @@
       </c>
       <c r="C6" s="73" t="str">
         <f aca="false">IF(ISBLANK(Main!$B6),"",Main!$B6)</f>
-        <v>age</v>
+        <v>number</v>
       </c>
       <c r="D6" s="99"/>
       <c r="E6" s="100"/>
@@ -35585,7 +35581,7 @@
       </c>
       <c r="C8" s="73" t="str">
         <f aca="false">IF(ISBLANK(Main!$B8),"",Main!$B8)</f>
-        <v>birth_date</v>
+        <v>date</v>
       </c>
       <c r="D8" s="99"/>
       <c r="E8" s="100"/>
@@ -35602,7 +35598,7 @@
       </c>
       <c r="C9" s="73" t="str">
         <f aca="false">IF(ISBLANK(Main!$B9),"",Main!$B9)</f>
-        <v>cities</v>
+        <v>dates</v>
       </c>
       <c r="D9" s="99"/>
       <c r="E9" s="100"/>
@@ -35619,7 +35615,7 @@
       </c>
       <c r="C10" s="73" t="str">
         <f aca="false">IF(ISBLANK(Main!$B6),"",Main!$B6)</f>
-        <v>age</v>
+        <v>number</v>
       </c>
       <c r="D10" s="99"/>
       <c r="E10" s="100"/>
@@ -35636,7 +35632,7 @@
       </c>
       <c r="C11" s="73" t="str">
         <f aca="false">IF(ISBLANK(Main!$B11),"",Main!$B11)</f>
-        <v/>
+        <v>bools</v>
       </c>
       <c r="D11" s="99"/>
       <c r="E11" s="100"/>

</xml_diff>

<commit_message>
Add fn transform_data with attribute mapping transformation
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -812,10 +812,16 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
+    <t xml:space="preserve">e-mail*</t>
+  </si>
+  <si>
     <t xml:space="preserve">licenses*</t>
   </si>
   <si>
     <t xml:space="preserve">A|B|C|D|E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a:A|b:B|c:C|d:D|e:E</t>
   </si>
   <si>
     <t xml:space="preserve">number</t>
@@ -1801,11 +1807,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2422,9 +2428,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>115560</xdr:colOff>
+      <xdr:colOff>114480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2438,7 +2444,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4061520" y="282960"/>
-          <a:ext cx="2895480" cy="815760"/>
+          <a:ext cx="2894400" cy="814680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4173,8 +4179,8 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4286,7 +4292,9 @@
         <v>94</v>
       </c>
       <c r="L4" s="69"/>
-      <c r="M4" s="70"/>
+      <c r="M4" s="70" t="s">
+        <v>95</v>
+      </c>
       <c r="N4" s="69"/>
       <c r="O4" s="71"/>
       <c r="P4" s="71"/>
@@ -4307,7 +4315,7 @@
         <v/>
       </c>
       <c r="B5" s="67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C5" s="74" t="s">
         <v>58</v>
@@ -4318,7 +4326,7 @@
       </c>
       <c r="F5" s="66"/>
       <c r="G5" s="66" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H5" s="67"/>
       <c r="I5" s="66"/>
@@ -4328,7 +4336,9 @@
       </c>
       <c r="L5" s="75"/>
       <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
+      <c r="N5" s="75" t="s">
+        <v>98</v>
+      </c>
       <c r="O5" s="76"/>
       <c r="P5" s="76"/>
       <c r="Q5" s="76"/>
@@ -4348,7 +4358,7 @@
         <v/>
       </c>
       <c r="B6" s="67" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C6" s="74" t="s">
         <v>66</v>
@@ -4385,7 +4395,7 @@
         <v/>
       </c>
       <c r="B7" s="77" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C7" s="74" t="s">
         <v>68</v>
@@ -4422,7 +4432,7 @@
         <v/>
       </c>
       <c r="B8" s="67" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C8" s="74" t="s">
         <v>60</v>
@@ -4432,7 +4442,7 @@
         <v>92</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G8" s="66"/>
       <c r="H8" s="67"/>
@@ -4461,7 +4471,7 @@
         <v/>
       </c>
       <c r="B9" s="67" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C9" s="74" t="s">
         <v>62</v>
@@ -4471,7 +4481,7 @@
         <v>92</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="67"/>
@@ -4500,7 +4510,7 @@
         <v/>
       </c>
       <c r="B10" s="67" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C10" s="74" t="s">
         <v>53</v>
@@ -4537,7 +4547,7 @@
         <v/>
       </c>
       <c r="B11" s="67" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C11" s="78" t="s">
         <v>55</v>
@@ -35410,10 +35420,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="50" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F1" s="86" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -35442,10 +35452,10 @@
       <c r="C2" s="88"/>
       <c r="D2" s="55"/>
       <c r="E2" s="89" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -35470,10 +35480,10 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="91" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Transform data from overlays passed in transform_data argument
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -812,16 +812,10 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">e-mail*</t>
-  </si>
-  <si>
     <t xml:space="preserve">licenses*</t>
   </si>
   <si>
     <t xml:space="preserve">A|B|C|D|E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a:A|b:B|c:C|d:D|e:E</t>
   </si>
   <si>
     <t xml:space="preserve">number</t>
@@ -2428,9 +2422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>114480</xdr:colOff>
+      <xdr:colOff>114120</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2444,7 +2438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4061520" y="282960"/>
-          <a:ext cx="2894400" cy="814680"/>
+          <a:ext cx="2894040" cy="814320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4292,9 +4286,7 @@
         <v>94</v>
       </c>
       <c r="L4" s="69"/>
-      <c r="M4" s="70" t="s">
-        <v>95</v>
-      </c>
+      <c r="M4" s="70"/>
       <c r="N4" s="69"/>
       <c r="O4" s="71"/>
       <c r="P4" s="71"/>
@@ -4315,7 +4307,7 @@
         <v/>
       </c>
       <c r="B5" s="67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="74" t="s">
         <v>58</v>
@@ -4326,7 +4318,7 @@
       </c>
       <c r="F5" s="66"/>
       <c r="G5" s="66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="67"/>
       <c r="I5" s="66"/>
@@ -4336,9 +4328,7 @@
       </c>
       <c r="L5" s="75"/>
       <c r="M5" s="75"/>
-      <c r="N5" s="75" t="s">
-        <v>98</v>
-      </c>
+      <c r="N5" s="75"/>
       <c r="O5" s="76"/>
       <c r="P5" s="76"/>
       <c r="Q5" s="76"/>
@@ -4358,7 +4348,7 @@
         <v/>
       </c>
       <c r="B6" s="67" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" s="74" t="s">
         <v>66</v>
@@ -4395,7 +4385,7 @@
         <v/>
       </c>
       <c r="B7" s="77" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" s="74" t="s">
         <v>68</v>
@@ -4432,7 +4422,7 @@
         <v/>
       </c>
       <c r="B8" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="74" t="s">
         <v>60</v>
@@ -4442,7 +4432,7 @@
         <v>92</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8" s="66"/>
       <c r="H8" s="67"/>
@@ -4471,7 +4461,7 @@
         <v/>
       </c>
       <c r="B9" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" s="74" t="s">
         <v>62</v>
@@ -4481,7 +4471,7 @@
         <v>92</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="67"/>
@@ -4510,7 +4500,7 @@
         <v/>
       </c>
       <c r="B10" s="67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="74" t="s">
         <v>53</v>
@@ -4547,7 +4537,7 @@
         <v/>
       </c>
       <c r="B11" s="67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C11" s="78" t="s">
         <v>55</v>
@@ -35420,10 +35410,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="86" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -35452,10 +35442,10 @@
       <c r="C2" s="88"/>
       <c r="D2" s="55"/>
       <c r="E2" s="89" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -35480,10 +35470,10 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="91" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Bump oca-rust to v0.2.1
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -830,10 +830,16 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
+    <t xml:space="preserve">DateTime</t>
+  </si>
+  <si>
     <t xml:space="preserve">DD.MM.YYYY</t>
   </si>
   <si>
     <t xml:space="preserve">dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array[DateTime]</t>
   </si>
   <si>
     <t xml:space="preserve">bool</t>
@@ -1708,7 +1714,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1804,11 +1810,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2425,9 +2431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>113400</xdr:colOff>
+      <xdr:colOff>113040</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2441,7 +2447,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4061520" y="282960"/>
-          <a:ext cx="2893320" cy="813600"/>
+          <a:ext cx="2892960" cy="813240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4177,7 +4183,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4430,14 +4436,14 @@
         <v>100</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D8" s="64"/>
       <c r="E8" s="65" t="s">
         <v>92</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G8" s="66"/>
       <c r="H8" s="67"/>
@@ -4466,17 +4472,17 @@
         <v/>
       </c>
       <c r="B9" s="67" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="D9" s="64"/>
       <c r="E9" s="65" t="s">
         <v>92</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="67"/>
@@ -4505,7 +4511,7 @@
         <v/>
       </c>
       <c r="B10" s="67" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C10" s="74" t="s">
         <v>53</v>
@@ -4542,7 +4548,7 @@
         <v/>
       </c>
       <c r="B11" s="67" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C11" s="78" t="s">
         <v>55</v>
@@ -35415,10 +35421,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="50" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F1" s="86" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -35447,10 +35453,10 @@
       <c r="C2" s="88"/>
       <c r="D2" s="55"/>
       <c r="E2" s="89" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -35475,10 +35481,10 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="91" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>22</v>

</xml_diff>